<commit_message>
🎁 updated student tasks
</commit_message>
<xml_diff>
--- a/Dica's Microsoft Missions/StudentTasks/Practical Task Brief Slide 6.xlsx
+++ b/Dica's Microsoft Missions/StudentTasks/Practical Task Brief Slide 6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cancelcloud/Library/Mobile Documents/com~apple~CloudDocs/Schule/TKDV/Excel for dummies/Schüler Aufgaben/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52F3592-1B12-4540-92A0-CFB33739451F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EBEA13-C6D5-2B4C-A305-65FD42F74084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8520" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{D9534318-3A6E-B54A-8CF4-AEF81DC675A2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{D9534318-3A6E-B54A-8CF4-AEF81DC675A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabe" sheetId="2" r:id="rId1"/>
@@ -159,13 +159,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -483,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4229616-9001-E847-9EC0-6F2372B1E20A}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="386" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+    <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,16 +517,16 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="5">
         <v>2000</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>1500</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>200</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -532,16 +534,16 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>1800</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>1600</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>200</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -558,7 +560,7 @@
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -566,7 +568,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
@@ -620,16 +622,16 @@
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>